<commit_message>
added dialog box for user consent at board processing
</commit_message>
<xml_diff>
--- a/outs/strips1.xlsx
+++ b/outs/strips1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="258">
   <si>
     <t>image</t>
   </si>
@@ -67,742 +67,727 @@
     <t>offset_microns</t>
   </si>
   <si>
-    <t>['S088_999_999_999']</t>
-  </si>
-  <si>
-    <t>['S017_010_009_001', 'S027_003_011_002', 'S034_004_012_999', 'S042_014_999_999', 'S049_006_015_005', 'S059_017_016_007', 'S066_018_999_008']</t>
-  </si>
-  <si>
-    <t>['S015_020_030_019', 'S028_022_032_021', 'S043_024_999_013', 'S056_026_025_999', 'S069_028_038_027', 'S089_999_999_999']</t>
-  </si>
-  <si>
-    <t>['S010_999_041_029', 'S018_031_999_999', 'S039_034_033_023', 'S053_036_047_035', 'S063_049_048_037', 'S076_051_050_039']</t>
-  </si>
-  <si>
-    <t>['S005_053_052_040', 'S024_043_055_042', 'S035_045_999_044', 'S045_059_058_046', 'S070_999_063_999']</t>
-  </si>
-  <si>
-    <t>['S007_999_067_999', 'S011_054_999_999', 'S029_072_071_056', 'S050_075_074_999', 'S060_061_076_060', 'S064_062_999_999', 'S081_065_079_064', 'S082_080_999_999', 'S087_999_999_999']</t>
-  </si>
-  <si>
-    <t>['S002_082_081_066', 'S012_084_083_068', 'S019_070_999_999', 'S020_999_999_069', 'S036_073_087_999', 'S061_091_090_076', 'S071_078_092_077', 'S077_999_093_999']</t>
-  </si>
-  <si>
-    <t>['S001_999_096_999', 'S026_086_999_085', 'S044_104_103_088', 'S054_999_105_089', 'S084_999_999_094', 'S086_111_110_095']</t>
-  </si>
-  <si>
-    <t>['S003_113_112_097', 'S006_114_113_098', 'S016_999_999_099', 'S021_116_115_100', 'S030_102_117_101', 'S040_119_118_999', 'S065_107_122_106', 'S078_109_124_108', 'S085_126_999_125']</t>
-  </si>
-  <si>
-    <t>['S004_128_141_127', 'S031_132_146_131', 'S051_999_134_120', 'S057_136_135_121', 'S072_138_137_123', 'S083_140_155_139', 'S090_999_999_999']</t>
-  </si>
-  <si>
-    <t>['S008_142_999_999', 'S013_999_143_129', 'S022_045_144_130', 'S041_148_147_133', 'S062_151_165_150', 'S074_153_999_152', 'S079_154_999_999']</t>
-  </si>
-  <si>
-    <t>['S009_157_156_999', 'S025_159_171_158', 'S037_161_173_160', 'S046_163_999_999', 'S052_999_163_149', 'S055_176_175_164', 'S067_178_177_166', 'S075_179_999_167', 'S080_168_999_999']</t>
-  </si>
-  <si>
-    <t>['S014_170_180_169', 'S032_999_999_172', 'S047_999_999_174', 'S073_189_999_999', 'S092_999_999_999']</t>
-  </si>
-  <si>
-    <t>['S023_191_190_181', 'S033_183_192_182', 'S038_184_193_999', 'S048_195_194_185', 'S058_187_196_186', 'S068_198_197_188']</t>
-  </si>
-  <si>
-    <t>['S091_999_999_999']</t>
-  </si>
-  <si>
-    <t>['1099']</t>
-  </si>
-  <si>
-    <t>['2000', '1560', '1561', '2440', '1561', '2000', '2000']</t>
-  </si>
-  <si>
-    <t>['4198', '4198', '3319', '3318', '4198', '3528']</t>
-  </si>
-  <si>
-    <t>['5516', '4637', '4637', '5516', '5956', '5957']</t>
-  </si>
-  <si>
-    <t>['7274', '6835', '6835', '7274', '6837']</t>
-  </si>
-  <si>
-    <t>['8593', '8153', '8597', '8590', '8153', '7714', '8153', '8590', '8801']</t>
-  </si>
-  <si>
-    <t>['9911', '9911', '9032', '9913', '9472', '9912', '9472', '9472']</t>
-  </si>
-  <si>
-    <t>['11230', '10790', '11229', '10790', '10790', '11229']</t>
-  </si>
-  <si>
-    <t>['12546', '12546', '12108', '12548', '12109', '12546', '12108', '12108', '13429']</t>
-  </si>
-  <si>
-    <t>['14745', '14745', '13864', '13866', '13866', '14745', '14104']</t>
-  </si>
-  <si>
-    <t>['15625', '15185', '15185', '15182', '16065', '16065', '15625']</t>
-  </si>
-  <si>
-    <t>['16503', '17382', '17382', '16943', '16502', '17822', '17825', '17822', '16503']</t>
-  </si>
-  <si>
-    <t>['18702', '19141', '18701', '19141', '18494']</t>
-  </si>
-  <si>
-    <t>['20458', '20019', '20021', '20458', '20019', '20458']</t>
-  </si>
-  <si>
-    <t>['21361']</t>
-  </si>
-  <si>
-    <t>['15918']</t>
-  </si>
-  <si>
-    <t>['18712', '16421', '14906', '13321', '11861', '9578', '8055']</t>
-  </si>
-  <si>
-    <t>['19473', '16428', '13383', '10341', '7294', '6133']</t>
-  </si>
-  <si>
-    <t>['20234', '18712', '14144', '11100', '8816', '5774']</t>
-  </si>
-  <si>
-    <t>['21757', '17951', '14906', '12623', '7297']</t>
-  </si>
-  <si>
-    <t>['20995', '20234', '16433', '11861', '9578', '8754', '5010', '4250', '23678']</t>
-  </si>
-  <si>
-    <t>['23279', '20235', '18650', '18713', '14906', '9576', '7294', '5772']</t>
-  </si>
-  <si>
-    <t>['24040', '17189', '13383', '11100', '3488', '2725']</t>
-  </si>
-  <si>
-    <t>['23280', '21755', '19473', '18712', '16429', '14146', '8816', '5772', '3489']</t>
-  </si>
-  <si>
-    <t>['22518', '16428', '11864', '10339', '7294', '4249', '3339']</t>
-  </si>
-  <si>
-    <t>['20933', '20235', '18713', '14142', '9579', '6536', '5709']</t>
-  </si>
-  <si>
-    <t>['20995', '17951', '14906', '12560', '11859', '11100', '8054', '6533', '5772']</t>
-  </si>
-  <si>
-    <t>['20238', '16426', '12622', '7292', '20891']</t>
-  </si>
-  <si>
-    <t>['18712', '16428', '14907', '12621', '10339', '8054']</t>
-  </si>
-  <si>
-    <t>['10337']</t>
-  </si>
-  <si>
-    <t>[359]</t>
-  </si>
-  <si>
-    <t>[360, 363, 383, 361, 366, 368, 370]</t>
-  </si>
-  <si>
-    <t>[358, 358, 364, 366, 368, 371]</t>
-  </si>
-  <si>
-    <t>[359, 359, 360, 363, 367, 369]</t>
-  </si>
-  <si>
-    <t>[351, 361, 361, 364, 366]</t>
-  </si>
-  <si>
-    <t>[360, 360, 357, 369, 369, 384, 371, 370, 354]</t>
-  </si>
-  <si>
-    <t>[356, 357, 358, 356, 358, 364, 366, 367]</t>
-  </si>
-  <si>
-    <t>[358, 360, 364, 362, 370, 371]</t>
-  </si>
-  <si>
-    <t>[359, 361, 362, 363, 361, 365, 369, 371, 370]</t>
-  </si>
-  <si>
-    <t>[359, 357, 368, 367, 369, 371, 369]</t>
-  </si>
-  <si>
-    <t>[356, 361, 361, 367, 368, 369, 334]</t>
-  </si>
-  <si>
-    <t>[362, 366, 368, 363, 367, 370, 372, 372, 371]</t>
-  </si>
-  <si>
-    <t>[364, 365, 368, 370, 365]</t>
-  </si>
-  <si>
-    <t>[368, 365, 364, 368, 366, 372]</t>
-  </si>
-  <si>
-    <t>[370]</t>
-  </si>
-  <si>
-    <t>[341]</t>
-  </si>
-  <si>
-    <t>[358, 350, 317, 319, 319, 309, 303]</t>
-  </si>
-  <si>
-    <t>[369, 343, 325, 310, 295, 290]</t>
-  </si>
-  <si>
-    <t>[370, 358, 329, 311, 298, 283]</t>
-  </si>
-  <si>
-    <t>[380, 353, 332, 319, 286]</t>
-  </si>
-  <si>
-    <t>[374, 369, 338, 311, 299, 271, 276, 269, 401]</t>
-  </si>
-  <si>
-    <t>[393, 366, 329, 356, 331, 303, 288, 278]</t>
-  </si>
-  <si>
-    <t>[401, 347, 320, 304, 262, 258]</t>
-  </si>
-  <si>
-    <t>[394, 380, 362, 356, 339, 326, 291, 274, 260]</t>
-  </si>
-  <si>
-    <t>[385, 328, 309, 302, 283, 267, 259]</t>
-  </si>
-  <si>
-    <t>[363, 362, 353, 325, 295, 277, 260]</t>
-  </si>
-  <si>
-    <t>[369, 345, 325, 304, 307, 305, 291, 282, 276]</t>
-  </si>
-  <si>
-    <t>[360, 338, 308, 289, 370]</t>
-  </si>
-  <si>
-    <t>[346, 332, 322, 312, 296, 292]</t>
-  </si>
-  <si>
-    <t>[304]</t>
-  </si>
-  <si>
-    <t>[225]</t>
-  </si>
-  <si>
-    <t>[355, 358, 358, 281, 361, 363, 364]</t>
-  </si>
-  <si>
-    <t>[357, 353, 360, 363, 360, 302]</t>
-  </si>
-  <si>
-    <t>[354, 357, 354, 359, 362, 364]</t>
-  </si>
-  <si>
-    <t>[353, 358, 357, 359, 360]</t>
-  </si>
-  <si>
-    <t>[353, 354, 352, 361, 362, 476, 365, 367, 291]</t>
-  </si>
-  <si>
-    <t>[352, 353, 536, 352, 353, 359, 361, 362]</t>
-  </si>
-  <si>
-    <t>[352, 354, 357, 357, 363, 366]</t>
-  </si>
-  <si>
-    <t>[357, 356, 357, 357, 355, 359, 361, 363, 365]</t>
-  </si>
-  <si>
-    <t>[354, 355, 359, 360, 363, 364, 425]</t>
-  </si>
-  <si>
-    <t>[188, 356, 354, 360, 360, 363, 193]</t>
-  </si>
-  <si>
-    <t>[357, 360, 361, 518, 358, 363, 364, 366, 366]</t>
-  </si>
-  <si>
-    <t>[360, 357, 361, 363, 421]</t>
-  </si>
-  <si>
-    <t>[361, 359, 357, 362, 361, 365]</t>
-  </si>
-  <si>
-    <t>[488]</t>
-  </si>
-  <si>
-    <t>[329]</t>
-  </si>
-  <si>
-    <t>[330, 332, 325, 472, 319, 317, 317]</t>
-  </si>
-  <si>
-    <t>[333, 325, 322, 317, 309, 203]</t>
-  </si>
-  <si>
-    <t>[339, 334, 320, 314, 311, 306]</t>
-  </si>
-  <si>
-    <t>[342, 324, 320, 313, 301]</t>
-  </si>
-  <si>
-    <t>[339, 332, 317, 311, 309, 177, 300, 301, 471]</t>
-  </si>
-  <si>
-    <t>[346, 334, 376, 324, 316, 311, 305, 302]</t>
-  </si>
-  <si>
-    <t>[360, 321, 315, 309, 289, 288]</t>
-  </si>
-  <si>
-    <t>[350, 340, 325, 326, 318, 313, 305, 300, 289]</t>
-  </si>
-  <si>
-    <t>[342, 317, 304, 306, 299, 291, 180]</t>
-  </si>
-  <si>
-    <t>[279, 324, 324, 315, 303, 296, 266]</t>
-  </si>
-  <si>
-    <t>[328, 316, 311, 316, 307, 307, 306, 300, 300]</t>
-  </si>
-  <si>
-    <t>[320, 312, 310, 308, 439]</t>
-  </si>
-  <si>
-    <t>[318, 311, 308, 307, 307, 307]</t>
-  </si>
-  <si>
-    <t>[309]</t>
-  </si>
-  <si>
-    <t>[1085]</t>
-  </si>
-  <si>
-    <t>[1987, 1550, 1571, 2428, 1554, 1995, 1997]</t>
-  </si>
-  <si>
-    <t>[4183, 4183, 3310, 3311, 4193, 3526]</t>
-  </si>
-  <si>
-    <t>[5502, 4623, 4624, 5506, 5950, 5953]</t>
-  </si>
-  <si>
-    <t>[7252, 6823, 6823, 7265, 6830]</t>
-  </si>
-  <si>
-    <t>[8580, 8140, 8581, 8586, 8149, 7725, 8151, 8587, 8782]</t>
-  </si>
-  <si>
-    <t>[9894, 9895, 9017, 9896, 9457, 9903, 9465, 9466]</t>
-  </si>
-  <si>
-    <t>[11215, 10777, 11220, 10779, 10787, 11227]</t>
-  </si>
-  <si>
-    <t>[12532, 12534, 12097, 12538, 12097, 12538, 12104, 12106, 13426]</t>
-  </si>
-  <si>
-    <t>[14731, 14729, 13859, 13860, 13862, 14743, 14100]</t>
-  </si>
-  <si>
-    <t>[15608, 15173, 15173, 15176, 16060, 16061, 15586]</t>
-  </si>
-  <si>
-    <t>[16492, 17375, 17377, 16933, 16496, 17819, 17824, 17821, 16501]</t>
-  </si>
-  <si>
-    <t>[18693, 19133, 18696, 19138, 18486]</t>
-  </si>
-  <si>
-    <t>[20453, 20011, 20012, 20453, 20012, 20457]</t>
-  </si>
-  <si>
-    <t>[21358]</t>
-  </si>
-  <si>
-    <t>[15886]</t>
-  </si>
-  <si>
-    <t>[18697, 16398, 14850, 13267, 11807, 9514, 7985]</t>
-  </si>
-  <si>
-    <t>[19469, 16398, 13335, 10278, 7216, 6050]</t>
-  </si>
-  <si>
-    <t>[20231, 18697, 14100, 11038, 8741, 5684]</t>
-  </si>
-  <si>
-    <t>[21764, 17931, 14865, 12569, 7210]</t>
-  </si>
-  <si>
-    <t>[20996, 20230, 16398, 11799, 9504, 8652, 4913, 4146, 23706]</t>
-  </si>
-  <si>
-    <t>[23299, 20228, 18606, 18696, 14864, 9506, 7209, 5677]</t>
-  </si>
-  <si>
-    <t>[24068, 17163, 13330, 11031, 3377, 2610]</t>
-  </si>
-  <si>
-    <t>[23301, 21762, 19462, 18695, 16395, 14099, 8734, 5673, 3376]</t>
-  </si>
-  <si>
-    <t>[22530, 16383, 11800, 10268, 7204, 4143, 3225]</t>
-  </si>
-  <si>
-    <t>[20923, 20224, 18693, 14094, 9501, 6440, 5596]</t>
-  </si>
-  <si>
-    <t>[20991, 17923, 14858, 12491, 11793, 11032, 7972, 6442, 5675]</t>
-  </si>
-  <si>
-    <t>[20225, 16391, 12557, 7208, 20888]</t>
-  </si>
-  <si>
-    <t>[18685, 16387, 14856, 12560, 10262, 7973]</t>
-  </si>
-  <si>
-    <t>[10268]</t>
-  </si>
-  <si>
-    <t>[951]</t>
-  </si>
-  <si>
-    <t>[1982, 1545, 1546, 2348, 1549, 1990, 1991]</t>
-  </si>
-  <si>
-    <t>[4182, 4178, 3306, 3308, 4185, 3457]</t>
-  </si>
-  <si>
-    <t>[5497, 4621, 4618, 5502, 5945, 5948]</t>
-  </si>
-  <si>
-    <t>[7254, 6820, 6819, 7260, 6824]</t>
-  </si>
-  <si>
-    <t>[8573, 8134, 8576, 8578, 8142, 7817, 8145, 8584, 8719]</t>
-  </si>
-  <si>
-    <t>[9890, 9891, 9195, 9892, 9452, 9898, 9460, 9461]</t>
-  </si>
-  <si>
-    <t>[11209, 10771, 11213, 10774, 10780, 11222]</t>
-  </si>
-  <si>
-    <t>[12530, 12529, 12092, 12532, 12091, 12532, 12096, 12098, 13421]</t>
-  </si>
-  <si>
-    <t>[14726, 14727, 13850, 13853, 13856, 14736, 14156]</t>
-  </si>
-  <si>
-    <t>[15440, 15168, 15166, 15169, 16052, 16055, 15445]</t>
-  </si>
-  <si>
-    <t>[16487, 17369, 17370, 17088, 16487, 17812, 17816, 17815, 16496]</t>
-  </si>
-  <si>
-    <t>[18689, 19125, 18689, 19131, 18542]</t>
-  </si>
-  <si>
-    <t>[20446, 20005, 20005, 20447, 20007, 20450]</t>
-  </si>
-  <si>
-    <t>[21476]</t>
-  </si>
-  <si>
-    <t>[15874]</t>
-  </si>
-  <si>
-    <t>[18669, 16380, 14858, 13420, 11807, 9522, 7999]</t>
-  </si>
-  <si>
-    <t>[19433, 16380, 13332, 10285, 7230, 5963]</t>
-  </si>
-  <si>
-    <t>[20200, 18673, 14091, 11041, 8754, 5707]</t>
-  </si>
-  <si>
-    <t>[21726, 17902, 14853, 12563, 7225]</t>
-  </si>
-  <si>
-    <t>[20961, 20193, 16377, 11799, 9514, 8558, 4937, 4178, 23776]</t>
-  </si>
-  <si>
-    <t>[23252, 20196, 18653, 18664, 14849, 9514, 7226, 5701]</t>
-  </si>
-  <si>
-    <t>[24027, 17137, 13325, 11036, 3404, 2640]</t>
-  </si>
-  <si>
-    <t>[23257, 21722, 19425, 18665, 16374, 14086, 8748, 5699, 3405]</t>
-  </si>
-  <si>
-    <t>[22487, 16372, 11795, 10272, 7220, 4167, 3146]</t>
-  </si>
-  <si>
-    <t>[20839, 20186, 18664, 14084, 9509, 6459, 5602]</t>
-  </si>
-  <si>
-    <t>[20950, 17894, 14844, 12503, 11793, 11034, 7987, 6460, 5699]</t>
-  </si>
-  <si>
-    <t>[20185, 16365, 12559, 7227, 20957]</t>
-  </si>
-  <si>
-    <t>[18657, 16366, 14842, 12555, 10273, 7988]</t>
-  </si>
-  <si>
-    <t>[10273]</t>
-  </si>
-  <si>
-    <t>[-11.0]</t>
-  </si>
-  <si>
-    <t>[-4.0, -7.0, -7.0, 0.0, -7.0, -4.0, -4.0]</t>
-  </si>
-  <si>
-    <t>[13.0, 13.0, 7.0, 7.0, 14.0, 8.0]</t>
-  </si>
-  <si>
-    <t>[24.0, 17.0, 17.0, 24.0, 27.0, 27.0]</t>
-  </si>
-  <si>
-    <t>[38.0, 34.0, 34.0, 38.0, 34.0]</t>
-  </si>
-  <si>
-    <t>[48.0, 45.0, 48.0, 48.0, 45.0, 42.0, 45.0, 48.0, 50.0]</t>
-  </si>
-  <si>
-    <t>[59.0, 59.0, 52.0, 59.0, 55.0, 59.0, 55.0, 55.0]</t>
-  </si>
-  <si>
-    <t>[69.0, 66.0, 69.0, 66.0, 66.0, 69.0]</t>
-  </si>
-  <si>
-    <t>[80.0, 80.0, 76.0, 80.0, 76.0, 80.0, 76.0, 76.0, 87.0]</t>
-  </si>
-  <si>
-    <t>[97.0, 97.0, 90.0, 90.0, 90.0, 97.0, 92.0]</t>
-  </si>
-  <si>
-    <t>[104.0, 101.0, 101.0, 101.0, 108.0, 108.0, 104.0]</t>
-  </si>
-  <si>
-    <t>[111.0, 118.0, 118.0, 115.0, 111.0, 122.0, 122.0, 122.0, 111.0]</t>
-  </si>
-  <si>
-    <t>[129.0, 132.0, 129.0, 132.0, 127.0]</t>
-  </si>
-  <si>
-    <t>[143.0, 139.0, 139.0, 143.0, 139.0, 143.0]</t>
-  </si>
-  <si>
-    <t>[150.0]</t>
-  </si>
-  <si>
-    <t>[20.0]</t>
-  </si>
-  <si>
-    <t>[43.0, 24.0, 12.0, 0.0, -12.0, -30.0, -42.0]</t>
-  </si>
-  <si>
-    <t>[49.0, 24.0, 0.0, -24.0, -49.0, -58.0]</t>
-  </si>
-  <si>
-    <t>[55.0, 43.0, 6.0, -18.0, -36.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[67.0, 37.0, 12.0, -6.0, -49.0]</t>
-  </si>
-  <si>
-    <t>[61.0, 55.0, 24.0, -12.0, -30.0, -37.0, -67.0, -73.0, 82.0]</t>
-  </si>
-  <si>
-    <t>[79.0, 55.0, 42.0, 43.0, 12.0, -30.0, -49.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[85.0, 30.0, 0.0, -18.0, -79.0, -85.0]</t>
-  </si>
-  <si>
-    <t>[79.0, 67.0, 49.0, 43.0, 24.0, 6.0, -36.0, -61.0, -79.0]</t>
-  </si>
-  <si>
-    <t>[73.0, 24.0, -12.0, -24.0, -49.0, -73.0, -80.0]</t>
-  </si>
-  <si>
-    <t>[60.0, 55.0, 43.0, 6.0, -30.0, -55.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[61.0, 36.0, 12.0, -7.0, -12.0, -18.0, -43.0, -55.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[55.0, 24.0, -6.0, -49.0, 60.0]</t>
-  </si>
-  <si>
-    <t>[43.0, 24.0, 12.0, -6.0, -24.0, -43.0]</t>
-  </si>
-  <si>
-    <t>[-24.0]</t>
-  </si>
-  <si>
-    <t>[-12.0]</t>
-  </si>
-  <si>
-    <t>[-4.0, -8.0, -8.0, -1.0, -7.0, -4.0, -4.0]</t>
-  </si>
-  <si>
-    <t>[13.0, 13.0, 6.0, 6.0, 13.0, 8.0]</t>
-  </si>
-  <si>
-    <t>[48.0, 45.0, 48.0, 48.0, 45.0, 42.0, 45.0, 48.0, 49.0]</t>
-  </si>
-  <si>
-    <t>[59.0, 59.0, 53.0, 59.0, 55.0, 59.0, 55.0, 55.0]</t>
-  </si>
-  <si>
-    <t>[97.0, 97.0, 90.0, 90.0, 90.0, 97.0, 93.0]</t>
-  </si>
-  <si>
-    <t>[103.0, 101.0, 101.0, 101.0, 108.0, 108.0, 103.0]</t>
-  </si>
-  <si>
-    <t>[111.0, 118.0, 118.0, 116.0, 111.0, 122.0, 122.0, 122.0, 111.0]</t>
-  </si>
-  <si>
-    <t>[151.0]</t>
-  </si>
-  <si>
-    <t>[42.0, 24.0, 12.0, 1.0, -12.0, -30.0, -42.0]</t>
-  </si>
-  <si>
-    <t>[48.0, 24.0, 0.0, -24.0, -48.0, -58.0]</t>
-  </si>
-  <si>
-    <t>[55.0, 42.0, 6.0, -18.0, -36.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[67.0, 36.0, 12.0, -6.0, -48.0]</t>
-  </si>
-  <si>
-    <t>[61.0, 54.0, 24.0, -12.0, -30.0, -38.0, -67.0, -73.0, 83.0]</t>
-  </si>
-  <si>
-    <t>[79.0, 54.0, 42.0, 42.0, 12.0, -30.0, -48.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[79.0, 67.0, 48.0, 42.0, 24.0, 6.0, -36.0, -61.0, -79.0]</t>
-  </si>
-  <si>
-    <t>[73.0, 24.0, -12.0, -24.0, -48.0, -73.0, -81.0]</t>
-  </si>
-  <si>
-    <t>[60.0, 54.0, 42.0, 6.0, -30.0, -55.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[60.0, 36.0, 12.0, -7.0, -12.0, -18.0, -42.0, -55.0, -61.0]</t>
-  </si>
-  <si>
-    <t>[54.0, 24.0, -6.0, -48.0, 61.0]</t>
-  </si>
-  <si>
-    <t>[42.0, 24.0, 12.0, -6.0, -24.0, -42.0]</t>
-  </si>
-  <si>
-    <t>[134.5362404707371]</t>
-  </si>
-  <si>
-    <t>[28.442925306655784, 18.681541692269406, 26.248809496813376, 172.6528308484978, 5.0, 9.433981132056603, 15.231546211727817]</t>
-  </si>
-  <si>
-    <t>[36.013886210738214, 18.681541692269406, 5.0, 7.615773105863909, 16.1245154965971, 111.04053313993049]</t>
-  </si>
-  <si>
-    <t>[31.400636936215164, 24.08318915758459, 10.816653826391969, 5.0, 13.92838827718412, 23.53720459187964]</t>
-  </si>
-  <si>
-    <t>[38.05259518088089, 29.154759474226502, 12.649110640673518, 7.810249675906654, 16.15549442140351]</t>
-  </si>
-  <si>
-    <t>[35.6931365951495, 37.48332962798263, 21.587033144922902, 8.0, 12.206555615733702, 131.52946437965906, 24.73863375370596, 32.14031735997639, 94.17536832951598]</t>
-  </si>
-  <si>
-    <t>[47.16990566028302, 32.2490309931942, 184.10051602317685, 32.2490309931942, 15.811388300841896, 9.433981132056603, 17.72004514666935, 24.515301344262525]</t>
-  </si>
-  <si>
-    <t>[41.43669871020132, 26.68332812825267, 8.602325267042627, 7.0710678118654755, 27.892651361962706, 30.4138126514911]</t>
-  </si>
-  <si>
-    <t>[44.04543109109048, 40.311288741492746, 37.33630940518894, 30.59411708155671, 21.840329667841555, 14.317821063276353, 16.1245154965971, 27.202941017470888, 29.427877939124322]</t>
-  </si>
-  <si>
-    <t>[43.289721643826724, 11.180339887498949, 10.295630140987, 8.06225774829855, 17.08800749063506, 25.0, 96.83491106000976]</t>
-  </si>
-  <si>
-    <t>[187.82971010998233, 38.3275357934736, 29.832867780352597, 12.206555615733702, 11.313708498984761, 19.924858845171276, 141.12760183606892]</t>
-  </si>
-  <si>
-    <t>[41.30375285612676, 29.614185789921695, 15.652475842498529, 155.46382215808282, 9.0, 7.280109889280518, 17.0, 18.973665961010276, 24.515301344262525]</t>
-  </si>
-  <si>
-    <t>[40.19950248448356, 27.202941017470888, 7.280109889280518, 20.248456731316587, 88.86506625215557]</t>
-  </si>
-  <si>
-    <t>[28.861739379323623, 21.840329667841555, 15.652475842498529, 7.810249675906654, 12.083045973594572, 16.55294535724685]</t>
-  </si>
-  <si>
-    <t>[118.10588469674151]</t>
-  </si>
-  <si>
-    <t>[1067.8814087364758]</t>
-  </si>
-  <si>
-    <t>[225.76571962158027, 148.2847371823884, 208.34992538095617, 1370.4318448599515, 39.6875, 74.8822252356993, 120.90039805558956]</t>
-  </si>
-  <si>
-    <t>[285.86022179773454, 148.2847371823884, 39.6875, 60.45019902779478, 127.98834175423946, 881.3842317981984]</t>
-  </si>
-  <si>
-    <t>[249.24255568120785, 191.1603139383277, 85.85718974698626, 39.6875, 110.55658195014894, 186.82656144804463]</t>
-  </si>
-  <si>
-    <t>[302.04247424824206, 231.41590332667286, 100.40231571034604, 61.993856802509065, 128.23423696989036]</t>
-  </si>
-  <si>
-    <t>[283.3142717239991, 297.5239289221121, 171.34707558782554, 63.5, 96.88953519988627, 1044.0151235135438, 196.36290542004107, 255.1137690448126, 747.5169861155331]</t>
-  </si>
-  <si>
-    <t>[374.4111261784965, 255.9766835084789, 1461.297845933966, 255.9766835084789, 125.50289463793256, 74.8822252356993, 140.65285835168797, 194.59020442008378]</t>
-  </si>
-  <si>
-    <t>[328.903796012223, 211.79891701800557, 68.28095680715086, 56.12660075668221, 221.39792018557898, 241.4096379212106]</t>
-  </si>
-  <si>
-    <t>[349.61060928553064, 319.97085438559867, 296.3569559036872, 242.84080433485641, 173.35761673849237, 113.64770468975604, 127.98834175423946, 215.92334432617517, 233.5837811417993]</t>
-  </si>
-  <si>
-    <t>[343.6121655478746, 88.7439478570229, 81.72156424408432, 63.99417087711973, 135.6360594569158, 198.4375, 768.6271065388275]</t>
-  </si>
-  <si>
-    <t>[1490.8983239979848, 304.2248153606967, 236.79838800654875, 96.88953519988627, 89.80256121069155, 158.15356708354702, 1120.200339573797]</t>
-  </si>
-  <si>
-    <t>[327.84853829550616, 235.06259970750347, 124.24152699983208, 1233.9940883797824, 71.4375, 57.78587224616411, 134.9375, 150.60347356551907, 194.59020442008378]</t>
-  </si>
-  <si>
-    <t>[319.08355097058825, 215.92334432617517, 57.78587224616411, 160.7221253048254, 705.366463376485]</t>
-  </si>
-  <si>
-    <t>[229.09005632338125, 173.35761673849237, 124.24152699983208, 61.993856802509065, 95.90917741540692, 131.38900377314684]</t>
-  </si>
-  <si>
-    <t>[937.4654597803857]</t>
+    <t>['S001_999_096_999', 'S002_082_081_066', 'S003_113_112_097', 'S087_999_999_999']</t>
+  </si>
+  <si>
+    <t>['S004_128_141_127', 'S005_053_052_040', 'S006_114_113_098']</t>
+  </si>
+  <si>
+    <t>['S007_999_067_999', 'S008_142_999_999', 'S009_157_156_999', 'S010_999_041_029', 'S011_054_999_999', 'S012_084_083_068', 'S013_999_143_129', 'S014_170_180_169', 'S092_999_999_999']</t>
+  </si>
+  <si>
+    <t>['S015_020_030_019', 'S016_999_999_099', 'S017_010_009_001', 'S018_031_999_999', 'S019_070_999_999', 'S020_999_999_069', 'S021_116_115_100', 'S022_045_144_130', 'S023_191_190_181']</t>
+  </si>
+  <si>
+    <t>['S024_043_055_042', 'S025_159_171_158', 'S026_086_999_085']</t>
+  </si>
+  <si>
+    <t>['S027_003_011_002', 'S028_022_032_021', 'S029_072_071_056', 'S030_102_117_101', 'S031_132_146_131', 'S032_999_999_172', 'S033_183_192_182', 'S088_999_999_999']</t>
+  </si>
+  <si>
+    <t>['S034_004_012_999', 'S035_045_999_044', 'S036_073_087_999', 'S037_161_173_160', 'S038_184_193_999', 'S039_034_033_023', 'S040_119_118_999', 'S041_148_147_133']</t>
+  </si>
+  <si>
+    <t>['S042_014_999_999', 'S043_024_999_013', 'S044_104_103_088', 'S045_059_058_046', 'S046_163_999_999', 'S047_999_999_174', 'S048_195_194_185']</t>
+  </si>
+  <si>
+    <t>['S049_006_015_005', 'S050_075_074_999', 'S051_999_134_120', 'S052_999_163_149', 'S053_036_047_035', 'S054_999_105_089', 'S055_176_175_164']</t>
+  </si>
+  <si>
+    <t>['S056_026_025_999', 'S057_136_135_121', 'S058_187_196_186', 'S059_017_016_007', 'S060_061_076_060', 'S061_091_090_076', 'S062_151_165_150', 'S091_999_999_999']</t>
+  </si>
+  <si>
+    <t>['S063_049_048_037', 'S064_062_999_999', 'S065_107_122_106', 'S066_018_999_008', 'S067_178_177_166', 'S068_198_197_188']</t>
+  </si>
+  <si>
+    <t>['S069_028_038_027', 'S070_999_063_999', 'S071_078_092_077', 'S072_138_137_123', 'S073_189_999_999', 'S074_153_999_152', 'S075_179_999_167']</t>
+  </si>
+  <si>
+    <t>['S076_051_050_039', 'S077_999_093_999', 'S078_109_124_108', 'S079_154_999_999', 'S080_168_999_999', 'S081_065_079_064', 'S089_999_999_999']</t>
+  </si>
+  <si>
+    <t>['S082_080_999_999', 'S083_140_155_139', 'S084_999_999_094', 'S085_126_999_125']</t>
+  </si>
+  <si>
+    <t>['S086_111_110_095', 'S090_999_999_999']</t>
+  </si>
+  <si>
+    <t>['1895', '2656', '2655', '2257']</t>
+  </si>
+  <si>
+    <t>['3417', '4178', '4180']</t>
+  </si>
+  <si>
+    <t>['4940', '5002', '4940', '5701', '5701', '5700', '5700', '5697', '5044']</t>
+  </si>
+  <si>
+    <t>['6462', '6462', '7223', '7223', '7285', '7222', '7223', '7222', '7223']</t>
+  </si>
+  <si>
+    <t>['7984', '7984', '8746']</t>
+  </si>
+  <si>
+    <t>['9514', '9507', '9502', '9506', '9507', '9509', '9507', '10017']</t>
+  </si>
+  <si>
+    <t>['11029', '11029', '11029', '11029', '11028', '11791', '11789', '11793']</t>
+  </si>
+  <si>
+    <t>['12614', '12552', '12552', '13312', '13375', '13313', '13314']</t>
+  </si>
+  <si>
+    <t>['14074', '14074', '14071', '14076', '14835', '14835', '14835']</t>
+  </si>
+  <si>
+    <t>['15594', '15596', '15596', '16357', '16357', '16359', '16356', '15598']</t>
+  </si>
+  <si>
+    <t>['17119', '17181', '17119', '17880', '17881', '17881']</t>
+  </si>
+  <si>
+    <t>['18641', '18638', '18641', '18641', '18643', '19399', '19402']</t>
+  </si>
+  <si>
+    <t>['20161', '20163', '20163', '20226', '20163', '20925', '19802']</t>
+  </si>
+  <si>
+    <t>['21685', '21686', '22447', '22446']</t>
+  </si>
+  <si>
+    <t>['23210', '22596']</t>
+  </si>
+  <si>
+    <t>['11230', '9911', '12546', '8801']</t>
+  </si>
+  <si>
+    <t>['14745', '7274', '12546']</t>
+  </si>
+  <si>
+    <t>['8593', '15625', '16503', '5516', '8153', '9911', '15185', '18702', '18494']</t>
+  </si>
+  <si>
+    <t>['4198', '12108', '2000', '4637', '9032', '9913', '12548', '15185', '20458']</t>
+  </si>
+  <si>
+    <t>['6835', '17382', '10790']</t>
+  </si>
+  <si>
+    <t>['1560', '4198', '8597', '12109', '14745', '19141', '20019', '1099']</t>
+  </si>
+  <si>
+    <t>['1561', '6835', '9472', '17382', '20021', '4637', '12546', '15182']</t>
+  </si>
+  <si>
+    <t>['2440', '3319', '11229', '7274', '16943', '18701', '20458']</t>
+  </si>
+  <si>
+    <t>['1561', '8590', '13864', '16502', '5516', '10790', '17822']</t>
+  </si>
+  <si>
+    <t>['3318', '13866', '20019', '2000', '8153', '9912', '16065', '21361']</t>
+  </si>
+  <si>
+    <t>['5956', '7714', '12108', '2000', '17825', '20458']</t>
+  </si>
+  <si>
+    <t>['4198', '6837', '9472', '13866', '19141', '16065', '17822']</t>
+  </si>
+  <si>
+    <t>['5957', '9472', '12108', '15625', '16503', '8153', '3528']</t>
+  </si>
+  <si>
+    <t>['8590', '14745', '10790', '13429']</t>
+  </si>
+  <si>
+    <t>['11229', '14104']</t>
+  </si>
+  <si>
+    <t>[295, 299, 313, 293]</t>
+  </si>
+  <si>
+    <t>[315, 324, 319]</t>
+  </si>
+  <si>
+    <t>[325, 337, 329, 329, 332, 328, 335, 344, 333]</t>
+  </si>
+  <si>
+    <t>[335, 338, 340, 337, 351, 344, 344, 346, 354]</t>
+  </si>
+  <si>
+    <t>[350, 353, 354]</t>
+  </si>
+  <si>
+    <t>[348, 353, 360, 360, 360, 366, 366, 359]</t>
+  </si>
+  <si>
+    <t>[364, 366, 368, 374, 376, 368, 376, 374]</t>
+  </si>
+  <si>
+    <t>[387, 374, 379, 381, 396, 386, 387]</t>
+  </si>
+  <si>
+    <t>[380, 387, 393, 388, 389, 394, 395]</t>
+  </si>
+  <si>
+    <t>[389, 397, 397, 389, 400, 398, 404, 395]</t>
+  </si>
+  <si>
+    <t>[402, 403, 406, 395, 409, 407]</t>
+  </si>
+  <si>
+    <t>[401, 413, 414, 416, 412, 422, 422]</t>
+  </si>
+  <si>
+    <t>[416, 423, 425, 421, 421, 425, 408]</t>
+  </si>
+  <si>
+    <t>[429, 431, 437, 435]</t>
+  </si>
+  <si>
+    <t>[442, 439]</t>
+  </si>
+  <si>
+    <t>[354, 356, 357, 358]</t>
+  </si>
+  <si>
+    <t>[359, 359, 362]</t>
+  </si>
+  <si>
+    <t>[360, 357, 365, 358, 357, 357, 361, 364, 364]</t>
+  </si>
+  <si>
+    <t>[358, 361, 360, 359, 361, 357, 364, 361, 366]</t>
+  </si>
+  <si>
+    <t>[361, 366, 360]</t>
+  </si>
+  <si>
+    <t>[363, 360, 357, 362, 362, 365, 365, 358]</t>
+  </si>
+  <si>
+    <t>[364, 362, 358, 367, 365, 361, 364, 367]</t>
+  </si>
+  <si>
+    <t>[365, 365, 363, 366, 363, 368, 369]</t>
+  </si>
+  <si>
+    <t>[364, 368, 368, 367, 364, 364, 361]</t>
+  </si>
+  <si>
+    <t>[367, 367, 368, 368, 366, 366, 367, 368]</t>
+  </si>
+  <si>
+    <t>[367, 364, 368, 370, 372, 371]</t>
+  </si>
+  <si>
+    <t>[368, 366, 367, 369, 371, 368, 369]</t>
+  </si>
+  <si>
+    <t>[369, 367, 372, 359, 371, 372, 369]</t>
+  </si>
+  <si>
+    <t>[371, 370, 369, 370]</t>
+  </si>
+  <si>
+    <t>[372, 369]</t>
+  </si>
+  <si>
+    <t>[341, 350, 348, 246]</t>
+  </si>
+  <si>
+    <t>[357, 362, 359]</t>
+  </si>
+  <si>
+    <t>[369, 370, 371, 366, 372, 369, 372, 376, 269]</t>
+  </si>
+  <si>
+    <t>[367, 373, 369, 371, 374, 375, 374, 378, 385]</t>
+  </si>
+  <si>
+    <t>[376, 383, 379]</t>
+  </si>
+  <si>
+    <t>[367, 375, 382, 382, 383, 388, 387, 370]</t>
+  </si>
+  <si>
+    <t>[375, 379, 380, 387, 390, 380, 386, 385]</t>
+  </si>
+  <si>
+    <t>[378, 376, 386, 385, 389, 391, 394]</t>
+  </si>
+  <si>
+    <t>[379, 388, 392, 392, 386, 390, 392]</t>
+  </si>
+  <si>
+    <t>[382, 394, 392, 382, 390, 389, 394, 390]</t>
+  </si>
+  <si>
+    <t>[390, 391, 393, 381, 393, 391]</t>
+  </si>
+  <si>
+    <t>[392, 394, 397, 396, 392, 403, 398]</t>
+  </si>
+  <si>
+    <t>[391, 397, 401, 397, 403, 400, 496]</t>
+  </si>
+  <si>
+    <t>[403, 406, 408, 410]</t>
+  </si>
+  <si>
+    <t>[410, 521]</t>
+  </si>
+  <si>
+    <t>[353, 353, 358, 281]</t>
+  </si>
+  <si>
+    <t>[354, 357, 356]</t>
+  </si>
+  <si>
+    <t>[354, 359, 359, 354, 354, 353, 355, 357, 415]</t>
+  </si>
+  <si>
+    <t>[353, 357, 354, 354, 354, 352, 357, 356, 360]</t>
+  </si>
+  <si>
+    <t>[359, 363, 352]</t>
+  </si>
+  <si>
+    <t>[357, 353, 352, 356, 355, 358, 358, 253]</t>
+  </si>
+  <si>
+    <t>[358, 356, 355, 361, 357, 355, 361, 360]</t>
+  </si>
+  <si>
+    <t>[360, 359, 355, 357, 360, 361, 362]</t>
+  </si>
+  <si>
+    <t>[362, 362, 361, 361, 358, 358, 363]</t>
+  </si>
+  <si>
+    <t>[363, 361, 362, 362, 361, 359, 359, 489]</t>
+  </si>
+  <si>
+    <t>[359, 362, 362, 366, 364, 364]</t>
+  </si>
+  <si>
+    <t>[365, 361, 360, 364, 365, 361, 366]</t>
+  </si>
+  <si>
+    <t>[366, 361, 363, 362, 364, 365, 298]</t>
+  </si>
+  <si>
+    <t>[365, 361, 362, 364]</t>
+  </si>
+  <si>
+    <t>[367, 426]</t>
+  </si>
+  <si>
+    <t>[1817, 2582, 2595, 2177]</t>
+  </si>
+  <si>
+    <t>[3359, 4129, 4126]</t>
+  </si>
+  <si>
+    <t>[4892, 4966, 4896, 5657, 5660, 5655, 5662, 5668, 5004]</t>
+  </si>
+  <si>
+    <t>[6424, 6427, 7190, 7187, 7263, 7193, 7194, 7195, 7204]</t>
+  </si>
+  <si>
+    <t>[7961, 7964, 8727]</t>
+  </si>
+  <si>
+    <t>[9489, 9487, 9489, 9493, 9494, 9502, 9500, 10003]</t>
+  </si>
+  <si>
+    <t>[11020, 11022, 11024, 11030, 11031, 11786, 11792, 11794]</t>
+  </si>
+  <si>
+    <t>[12628, 12553, 12558, 13320, 13398, 13326, 13328]</t>
+  </si>
+  <si>
+    <t>[14081, 14088, 14091, 14091, 14851, 14856, 14857]</t>
+  </si>
+  <si>
+    <t>[15610, 15620, 15620, 16373, 16384, 16384, 16387, 15620]</t>
+  </si>
+  <si>
+    <t>[17148, 17211, 17152, 17902, 17917, 17915]</t>
+  </si>
+  <si>
+    <t>[18669, 18678, 18682, 18684, 18682, 19448, 19451]</t>
+  </si>
+  <si>
+    <t>[20204, 20213, 20215, 20274, 20211, 20977, 19837]</t>
+  </si>
+  <si>
+    <t>[21741, 21744, 22511, 22508]</t>
+  </si>
+  <si>
+    <t>[23279, 22662]</t>
+  </si>
+  <si>
+    <t>[11211, 9894, 12530, 8786]</t>
+  </si>
+  <si>
+    <t>[14731, 7260, 12535]</t>
+  </si>
+  <si>
+    <t>[8580, 15609, 16495, 5501, 8137, 9895, 15173, 18693, 18485]</t>
+  </si>
+  <si>
+    <t>[4183, 12096, 1987, 4623, 9020, 9897, 12539, 15173, 20451]</t>
+  </si>
+  <si>
+    <t>[6823, 17375, 10777]</t>
+  </si>
+  <si>
+    <t>[1550, 4185, 8581, 12098, 14734, 19133, 20011, 1084]</t>
+  </si>
+  <si>
+    <t>[1552, 6824, 9457, 17376, 20013, 4625, 12537, 15176]</t>
+  </si>
+  <si>
+    <t>[2432, 3311, 11219, 7267, 16933, 18696, 20454]</t>
+  </si>
+  <si>
+    <t>[1552, 8585, 13859, 16496, 5507, 10781, 17810]</t>
+  </si>
+  <si>
+    <t>[3312, 13860, 20014, 1995, 8146, 9905, 16059, 21356]</t>
+  </si>
+  <si>
+    <t>[5950, 7705, 12103, 1997, 17824, 20456]</t>
+  </si>
+  <si>
+    <t>[4193, 6830, 9466, 13862, 19139, 16060, 17818]</t>
+  </si>
+  <si>
+    <t>[5953, 9466, 12107, 15611, 16501, 8152, 3524]</t>
+  </si>
+  <si>
+    <t>[8588, 14742, 10786, 13426]</t>
+  </si>
+  <si>
+    <t>[11228, 14100]</t>
+  </si>
+  <si>
+    <t>[1863, 2633, 2630, 2130]</t>
+  </si>
+  <si>
+    <t>[3401, 4167, 4166]</t>
+  </si>
+  <si>
+    <t>[4936, 4999, 4938, 5694, 5700, 5696, 5699, 5700, 4940]</t>
+  </si>
+  <si>
+    <t>[6456, 6462, 7219, 7221, 7286, 7224, 7224, 7227, 7235]</t>
+  </si>
+  <si>
+    <t>[7987, 7994, 8752]</t>
+  </si>
+  <si>
+    <t>[9508, 9509, 9511, 9515, 9517, 9524, 9521, 10014]</t>
+  </si>
+  <si>
+    <t>[11031, 11035, 11036, 11043, 11045, 11798, 11802, 11805]</t>
+  </si>
+  <si>
+    <t>[12619, 12555, 12565, 13324, 13391, 13331, 13335]</t>
+  </si>
+  <si>
+    <t>[14080, 14089, 14090, 14095, 14848, 14852, 14854]</t>
+  </si>
+  <si>
+    <t>[15603, 15617, 15615, 16366, 16374, 16375, 16377, 15615]</t>
+  </si>
+  <si>
+    <t>[17136, 17199, 17139, 17888, 17901, 17899]</t>
+  </si>
+  <si>
+    <t>[18660, 18659, 18665, 18664, 18662, 19429, 19427]</t>
+  </si>
+  <si>
+    <t>[20179, 20187, 20191, 20250, 20193, 20952, 19925]</t>
+  </si>
+  <si>
+    <t>[21715, 21719, 22482, 22483]</t>
+  </si>
+  <si>
+    <t>[23247, 22744]</t>
+  </si>
+  <si>
+    <t>[11210, 9891, 12531, 8709]</t>
+  </si>
+  <si>
+    <t>[14726, 7258, 12529]</t>
+  </si>
+  <si>
+    <t>[8574, 15611, 16489, 5497, 8134, 9891, 15167, 18686, 18536]</t>
+  </si>
+  <si>
+    <t>[4178, 12092, 1981, 4618, 9013, 9892, 12532, 15168, 20445]</t>
+  </si>
+  <si>
+    <t>[6821, 17372, 10769]</t>
+  </si>
+  <si>
+    <t>[1544, 4178, 8576, 12092, 14727, 19126, 20004, 979]</t>
+  </si>
+  <si>
+    <t>[1546, 6818, 9454, 17370, 20005, 4619, 12534, 15169]</t>
+  </si>
+  <si>
+    <t>[2427, 3305, 11211, 7258, 16930, 18689, 20447]</t>
+  </si>
+  <si>
+    <t>[1550, 8579, 13852, 16490, 5501, 10775, 17812]</t>
+  </si>
+  <si>
+    <t>[3308, 13854, 20008, 1989, 8141, 9898, 16051, 21477]</t>
+  </si>
+  <si>
+    <t>[5942, 7703, 12097, 1993, 17816, 20449]</t>
+  </si>
+  <si>
+    <t>[4190, 6825, 9459, 13857, 19133, 16053, 17815]</t>
+  </si>
+  <si>
+    <t>[5950, 9460, 12098, 15614, 16494, 8145, 3453]</t>
+  </si>
+  <si>
+    <t>[8582, 14733, 10779, 13420]</t>
+  </si>
+  <si>
+    <t>[11223, 14157]</t>
+  </si>
+  <si>
+    <t>[-86.0, -80.0, -80.0, -83.0]</t>
+  </si>
+  <si>
+    <t>[-74.0, -68.0, -68.0]</t>
+  </si>
+  <si>
+    <t>[-62.0, -61.0, -62.0, -56.0, -56.0, -56.0, -56.0, -56.0, -61.0]</t>
+  </si>
+  <si>
+    <t>[-50.0, -50.0, -44.0, -44.0, -43.0, -44.0, -44.0, -44.0, -44.0]</t>
+  </si>
+  <si>
+    <t>[-38.0, -38.0, -31.0]</t>
+  </si>
+  <si>
+    <t>[-25.0, -25.0, -25.0, -25.0, -25.0, -25.0, -25.0, -21.0]</t>
+  </si>
+  <si>
+    <t>[-13.0, -13.0, -13.0, -13.0, -13.0, -7.0, -7.0, -7.0]</t>
+  </si>
+  <si>
+    <t>[0.0, -1.0, -1.0, 5.0, 6.0, 5.0, 5.0]</t>
+  </si>
+  <si>
+    <t>[11.0, 11.0, 11.0, 11.0, 17.0, 17.0, 17.0]</t>
+  </si>
+  <si>
+    <t>[23.0, 23.0, 23.0, 29.0, 29.0, 29.0, 29.0, 23.0]</t>
+  </si>
+  <si>
+    <t>[35.0, 36.0, 35.0, 41.0, 41.0, 41.0]</t>
+  </si>
+  <si>
+    <t>[47.0, 48.0, 48.0, 48.0, 48.0, 54.0, 54.0]</t>
+  </si>
+  <si>
+    <t>[60.0, 60.0, 60.0, 60.0, 60.0, 66.0, 57.0]</t>
+  </si>
+  <si>
+    <t>[72.0, 72.0, 78.0, 78.0]</t>
+  </si>
+  <si>
+    <t>[84.0, 79.0]</t>
+  </si>
+  <si>
+    <t>[69.0, 59.0, 80.0, 50.0]</t>
+  </si>
+  <si>
+    <t>[97.0, 38.0, 80.0]</t>
+  </si>
+  <si>
+    <t>[48.0, 104.0, 111.0, 24.0, 45.0, 59.0, 101.0, 129.0, 127.0]</t>
+  </si>
+  <si>
+    <t>[13.0, 76.0, -4.0, 17.0, 52.0, 59.0, 80.0, 101.0, 143.0]</t>
+  </si>
+  <si>
+    <t>[34.0, 118.0, 66.0]</t>
+  </si>
+  <si>
+    <t>[-8.0, 13.0, 48.0, 76.0, 97.0, 132.0, 139.0, -11.0]</t>
+  </si>
+  <si>
+    <t>[-7.0, 34.0, 55.0, 118.0, 139.0, 17.0, 80.0, 101.0]</t>
+  </si>
+  <si>
+    <t>[0.0, 6.0, 69.0, 38.0, 115.0, 129.0, 143.0]</t>
+  </si>
+  <si>
+    <t>[-7.0, 48.0, 90.0, 111.0, 24.0, 66.0, 122.0]</t>
+  </si>
+  <si>
+    <t>[6.0, 90.0, 139.0, -4.0, 45.0, 59.0, 108.0, 150.0]</t>
+  </si>
+  <si>
+    <t>[27.0, 41.0, 76.0, -4.0, 122.0, 143.0]</t>
+  </si>
+  <si>
+    <t>[13.0, 34.0, 55.0, 90.0, 132.0, 108.0, 122.0]</t>
+  </si>
+  <si>
+    <t>[27.0, 55.0, 76.0, 104.0, 111.0, 45.0, 8.0]</t>
+  </si>
+  <si>
+    <t>[48.0, 97.0, 66.0, 87.0]</t>
+  </si>
+  <si>
+    <t>[69.0, 92.0]</t>
+  </si>
+  <si>
+    <t>[-86.0, -80.0, -80.0, -84.0]</t>
+  </si>
+  <si>
+    <t>[-62.0, -61.0, -62.0, -56.0, -55.0, -56.0, -55.0, -55.0, -62.0]</t>
+  </si>
+  <si>
+    <t>[-49.0, -49.0, -43.0, -43.0, -43.0, -43.0, -43.0, -43.0, -43.0]</t>
+  </si>
+  <si>
+    <t>[-37.0, -37.0, -31.0]</t>
+  </si>
+  <si>
+    <t>[-1.0, -1.0, -1.0, 5.0, 6.0, 5.0, 5.0]</t>
+  </si>
+  <si>
+    <t>[47.0, 47.0, 47.0, 47.0, 47.0, 53.0, 53.0]</t>
+  </si>
+  <si>
+    <t>[59.0, 59.0, 60.0, 60.0, 60.0, 66.0, 57.0]</t>
+  </si>
+  <si>
+    <t>[84.0, 80.0]</t>
+  </si>
+  <si>
+    <t>[69.0, 59.0, 80.0, 49.0]</t>
+  </si>
+  <si>
+    <t>[13.0, 76.0, -4.0, 17.0, 52.0, 59.0, 80.0, 101.0, 142.0]</t>
+  </si>
+  <si>
+    <t>[-8.0, 13.0, 48.0, 76.0, 97.0, 132.0, 139.0, -12.0]</t>
+  </si>
+  <si>
+    <t>[-8.0, 34.0, 55.0, 118.0, 139.0, 17.0, 80.0, 101.0]</t>
+  </si>
+  <si>
+    <t>[-1.0, 6.0, 69.0, 38.0, 115.0, 129.0, 142.0]</t>
+  </si>
+  <si>
+    <t>[-8.0, 48.0, 90.0, 111.0, 24.0, 66.0, 122.0]</t>
+  </si>
+  <si>
+    <t>[6.0, 90.0, 139.0, -4.0, 45.0, 59.0, 108.0, 151.0]</t>
+  </si>
+  <si>
+    <t>[69.0, 93.0]</t>
+  </si>
+  <si>
+    <t>[46.010868281309364, 51.088159097779204, 35.014282800023196, 90.21086409075129]</t>
+  </si>
+  <si>
+    <t>[42.2965719651132, 38.05259518088089, 40.44749683231337]</t>
+  </si>
+  <si>
+    <t>[44.40720662234904, 33.06055050963308, 42.42640687119285, 37.21558813185679, 40.11234224026316, 41.19465984809196, 37.48332962798263, 32.7566787083184, 81.83520025025906]</t>
+  </si>
+  <si>
+    <t>[32.38826948140329, 35.22782990761707, 29.614185789921695, 34.36568055487916, 24.041630560342615, 31.400636936215164, 30.805843601498726, 32.38826948140329, 31.575306807693888]</t>
+  </si>
+  <si>
+    <t>[26.076809620810597, 30.14962686336267, 26.248809496813376]</t>
+  </si>
+  <si>
+    <t>[19.924858845171276, 23.08679276123039, 22.561028345356956, 22.80350850198276, 24.041630560342615, 23.08679276123039, 22.135943621178654, 105.57461816175325]</t>
+  </si>
+  <si>
+    <t>[12.529964086141668, 14.317821063276353, 12.36931687685298, 14.317821063276353, 16.1245154965971, 13.416407864998739, 10.44030650891055, 13.038404810405298]</t>
+  </si>
+  <si>
+    <t>[10.295630140987, 6.324555320336759, 10.63014581273465, 9.848857801796104, 7.615773105863909, 8.602325267042627, 9.899494936611665]</t>
+  </si>
+  <si>
+    <t>[2.23606797749979, 6.082762530298219, 7.0710678118654755, 7.211102550927978, 6.708203932499369, 7.211102550927978, 3.605551275463989]</t>
+  </si>
+  <si>
+    <t>[8.06225774829855, 6.708203932499369, 7.810249675906654, 9.219544457292887, 11.180339887498949, 11.40175425099138, 12.806248474865697, 121.10326172320876]</t>
+  </si>
+  <si>
+    <t>[14.422205101855956, 12.165525060596439, 14.317821063276353, 14.560219778561036, 17.88854381999832, 17.46424919657298]</t>
+  </si>
+  <si>
+    <t>[9.486832980505138, 19.6468827043885, 18.384776310850235, 20.615528128088304, 20.8806130178211, 20.248456731316587, 24.186773244895647]</t>
+  </si>
+  <si>
+    <t>[25.179356624028344, 26.68332812825267, 25.632011235952593, 24.186773244895647, 19.313207915827967, 25.96150997149434, 113.07077429645558]</t>
+  </si>
+  <si>
+    <t>[26.68332812825267, 26.570660511172846, 29.832867780352597, 25.709920264364882]</t>
+  </si>
+  <si>
+    <t>[32.38826948140329, 99.86490875177326]</t>
+  </si>
+  <si>
+    <t>[365.21126698289305, 405.5122628386224, 277.92586972518416, 716.0487337203383]</t>
+  </si>
+  <si>
+    <t>[335.72903997308606, 302.04247424824206, 321.0520061064874]</t>
+  </si>
+  <si>
+    <t>[352.4822025648955, 262.4181196702126, 336.7596045400933, 295.3987307966133, 318.3917165320888, 326.98261254422994, 297.5239289221121, 260.00613724727725, 649.5669019864313]</t>
+  </si>
+  <si>
+    <t>[257.08188900863865, 279.6208998917105, 235.06259970750347, 272.77758940435336, 190.8304425727195, 249.24255568120785, 244.52138358689615, 257.08188900863865, 250.62899778607024]</t>
+  </si>
+  <si>
+    <t>[206.9846763651841, 239.3126632279412, 208.34992538095617]</t>
+  </si>
+  <si>
+    <t>[158.15356708354702, 183.25141754226624, 179.07816249127086, 181.00284873448814, 190.8304425727195, 183.25141754226624, 175.70405249310556, 837.9985316589165]</t>
+  </si>
+  <si>
+    <t>[99.4565899337495, 113.64770468975604, 98.18145271002054, 113.64770468975604, 127.98834175423946, 106.49273742842747, 82.8699329144775, 103.49233818259205]</t>
+  </si>
+  <si>
+    <t>[81.72156424408432, 50.20115785517302, 84.37678238858129, 78.17530880175657, 60.45019902779478, 68.28095680715086, 78.57724105935509]</t>
+  </si>
+  <si>
+    <t>[17.748789571404583, 48.28192758424211, 56.12660075668221, 57.23812649799083, 53.24636871421374, 57.23812649799083, 28.619063248995413]</t>
+  </si>
+  <si>
+    <t>[63.99417087711973, 53.24636871421374, 61.993856802509065, 73.1801341297623, 88.7439478570229, 90.50142436724407, 101.64959726924648, 961.2571399279695]</t>
+  </si>
+  <si>
+    <t>[114.47625299598165, 96.56385516848422, 113.64770468975604, 115.57174449232822, 141.99031657123666, 138.622477997798]</t>
+  </si>
+  <si>
+    <t>[75.30173678275953, 155.94713146608373, 145.92916196737374, 163.6357545167009, 165.739865828955, 160.7221253048254, 191.9825126313592]</t>
+  </si>
+  <si>
+    <t>[199.86114320322497, 211.79891701800557, 203.4540891853737, 191.9825126313592, 153.29858783188448, 206.06948539873633, 897.4992709781161]</t>
+  </si>
+  <si>
+    <t>[211.79891701800557, 210.90461780743448, 236.79838800654875, 204.07249209839625]</t>
+  </si>
+  <si>
+    <t>[257.08188900863865, 792.6777132172002]</t>
   </si>
 </sst>
 </file>
@@ -1266,13 +1251,13 @@
         <v>212</v>
       </c>
       <c r="P2" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="Q2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="R2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1319,16 +1304,16 @@
         <v>198</v>
       </c>
       <c r="O3" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="P3" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="Q3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="R3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1375,16 +1360,16 @@
         <v>199</v>
       </c>
       <c r="O4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P4" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="Q4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="R4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1431,16 +1416,16 @@
         <v>200</v>
       </c>
       <c r="O5" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="P5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="R5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1487,16 +1472,16 @@
         <v>201</v>
       </c>
       <c r="O6" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="P6" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="Q6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="R6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1543,16 +1528,16 @@
         <v>202</v>
       </c>
       <c r="O7" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="P7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="Q7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="R7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1599,16 +1584,16 @@
         <v>203</v>
       </c>
       <c r="O8" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="P8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Q8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="R8" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1655,16 +1640,16 @@
         <v>204</v>
       </c>
       <c r="O9" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="P9" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="Q9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="R9" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1714,13 +1699,13 @@
         <v>190</v>
       </c>
       <c r="P10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q10" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="R10" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1767,16 +1752,16 @@
         <v>206</v>
       </c>
       <c r="O11" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="P11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q11" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="R11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1823,16 +1808,16 @@
         <v>207</v>
       </c>
       <c r="O12" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="P12" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="Q12" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="R12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1879,16 +1864,16 @@
         <v>208</v>
       </c>
       <c r="O13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P13" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="Q13" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="R13" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1935,16 +1920,16 @@
         <v>209</v>
       </c>
       <c r="O14" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="P14" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="Q14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="R14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1994,13 +1979,13 @@
         <v>195</v>
       </c>
       <c r="P15" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="Q15" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="R15" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -2047,16 +2032,16 @@
         <v>211</v>
       </c>
       <c r="O16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P16" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="Q16" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="R16" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>